<commit_message>
my all commits for project date 1-7-2020
</commit_message>
<xml_diff>
--- a/public/demo/studentrec.xlsx
+++ b/public/demo/studentrec.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\laravel\Evento\public\demo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B20E2CE-B177-43A8-9674-2C75135A6471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="810" windowWidth="19575" windowHeight="7080"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,80 +20,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>E17111950110151</t>
   </si>
   <si>
-    <t>jay</t>
-  </si>
-  <si>
     <t>tybca</t>
   </si>
   <si>
-    <t>j@gmail.com</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
     <t>E17111950110152</t>
   </si>
   <si>
-    <t>raj</t>
-  </si>
-  <si>
-    <t>p@gmail.com</t>
-  </si>
-  <si>
     <t>E17111950110153</t>
   </si>
   <si>
-    <t>yash</t>
-  </si>
-  <si>
-    <t>y@gmail.com</t>
-  </si>
-  <si>
     <t>E17111950110154</t>
   </si>
   <si>
-    <t>parth</t>
-  </si>
-  <si>
-    <t>a@gmail.com</t>
-  </si>
-  <si>
     <t>female</t>
   </si>
   <si>
     <t>E17111950110155</t>
   </si>
   <si>
-    <t>neha</t>
-  </si>
-  <si>
-    <t>piyush@gmail.com</t>
-  </si>
-  <si>
     <t>E17111950110156</t>
   </si>
   <si>
-    <t>shivani</t>
-  </si>
-  <si>
-    <t>shivu@gmail.com</t>
-  </si>
-  <si>
     <t>E17111950110157</t>
   </si>
   <si>
-    <t>rushali</t>
-  </si>
-  <si>
-    <t>rushu@gmail.com</t>
-  </si>
-  <si>
     <t>240,bhagirath-2,l.h.road surat</t>
   </si>
   <si>
@@ -119,16 +83,76 @@
   </si>
   <si>
     <t>Gender</t>
+  </si>
+  <si>
+    <t>patel jay rajubhai</t>
+  </si>
+  <si>
+    <t>ramani raj maheshbhai</t>
+  </si>
+  <si>
+    <t>parmar yash kishorbhai</t>
+  </si>
+  <si>
+    <t>patthar parth maganbhai</t>
+  </si>
+  <si>
+    <t>vaghela neha rajubhai</t>
+  </si>
+  <si>
+    <t>patel shivani rameshbhai</t>
+  </si>
+  <si>
+    <t>paghdal maulik haribhai</t>
+  </si>
+  <si>
+    <t>24,panchvati society-2,l.h.road surat</t>
+  </si>
+  <si>
+    <t>A 240,Apple society-2,l.h.road surat</t>
+  </si>
+  <si>
+    <t>B40,ranjeet-2,l.h.road surat</t>
+  </si>
+  <si>
+    <t>121,tirupati-2,l.h.road surat</t>
+  </si>
+  <si>
+    <t>20,vrundavan-2,l.h.road surat</t>
+  </si>
+  <si>
+    <t>59,laxmi nagar-2,l.h.road surat</t>
+  </si>
+  <si>
+    <t>jayp1999p@gmail.com</t>
+  </si>
+  <si>
+    <t>rajramani2011999@gmail.com</t>
+  </si>
+  <si>
+    <t>parmaryash2000y@gmail.com</t>
+  </si>
+  <si>
+    <t>parthpatthar0070@gmail.com</t>
+  </si>
+  <si>
+    <t>neharvaghela199907@gmail.com</t>
+  </si>
+  <si>
+    <t>shivu007patel@gmail.com</t>
+  </si>
+  <si>
+    <t>maulikpaghdal111007@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -144,6 +168,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,10 +193,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -180,12 +211,22 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -386,60 +427,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="9" max="9" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3">
         <v>101</v>
@@ -448,217 +491,226 @@
         <v>36195</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="3">
+        <v>8033163874</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3">
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="3">
-        <v>9033163874</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3">
         <v>102</v>
       </c>
       <c r="D3" s="5">
-        <v>36195</v>
+        <v>36499</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
         <v>2</v>
       </c>
-      <c r="F3" s="3">
-        <v>3</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
+      <c r="G3" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="H3" s="3">
-        <v>9033163875</v>
+        <v>7033163875</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C4" s="4">
         <v>102</v>
       </c>
       <c r="D4" s="5">
-        <v>36195</v>
+        <v>36568</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="3">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
+      <c r="G4" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="H4" s="3">
-        <v>9033163876</v>
+        <v>9933163876</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="3">
         <v>104</v>
       </c>
       <c r="D5" s="5">
-        <v>36195</v>
+        <v>36383</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="4">
+        <v>8833163211</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="3">
-        <v>3</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="4">
-        <v>9033163211</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3">
         <v>105</v>
       </c>
       <c r="D6" s="5">
-        <v>36195</v>
+        <v>36199</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3">
-        <v>3</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="H6" s="3">
-        <v>9033163878</v>
+        <v>7733163878</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3">
         <v>106</v>
       </c>
       <c r="D7" s="5">
-        <v>36195</v>
+        <v>36498</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
         <v>2</v>
       </c>
-      <c r="F7" s="3">
-        <v>3</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>20</v>
+      <c r="G7" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="H7" s="3">
-        <v>9033163879</v>
+        <v>8933163879</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3">
         <v>107</v>
       </c>
       <c r="D8" s="5">
-        <v>36195</v>
+        <v>36560</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3">
         <v>3</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>23</v>
+      <c r="G8" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="H8" s="3">
-        <v>9033163880</v>
+        <v>9433163880</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{57833025-B008-45C2-9C5C-12378928EB81}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{428892B5-B008-430F-88BE-08AE353F8264}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{B860F7E5-6BE1-4DE3-AD67-BD0E058A41AA}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{E193EE1D-071C-4798-B042-F4B428BC143E}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{E6A2389B-8AF4-40DC-B68D-B945F4578CF3}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{B10BA0D1-D11F-4343-A826-65D23D8975C5}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{0EF00EEB-6F28-42AC-806D-AED29D5333F1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>